<commit_message>
Update FM5 worked example spreadsheet
</commit_message>
<xml_diff>
--- a/ftest/data/fm5/Worked_example_policy_calculation_3.xlsx
+++ b/ftest/data/fm5/Worked_example_policy_calculation_3.xlsx
@@ -4775,7 +4775,7 @@
     <mergeCell ref="C40:F40"/>
   </mergeCells>
   <pageMargins left="0.708661" right="0.708661" top="0.748031" bottom="0.748031" header="0.314961" footer="0.314961"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="44" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri,Bold"&amp;14&amp;K000000Format 3</oddHeader>
     <oddFooter>&amp;L&amp;"Calibri,Regular"&amp;11&amp;K00000013/11/2018&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P&amp;R&amp;"Calibri,Regular"&amp;11&amp;K000000FM5_Worked_example_policy_calculation_3.xlsx</oddFooter>
@@ -6692,7 +6692,7 @@
         <v>0</v>
       </c>
       <c r="V12" s="82">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="W12" s="82">
         <v>0</v>

</xml_diff>